<commit_message>
fixed bug in grid gen, cleaned up code for bigger solver
</commit_message>
<xml_diff>
--- a/ref/overlap_calculator.xlsx
+++ b/ref/overlap_calculator.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\Documents\wadl\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEE592F-85A5-48AD-968F-A3F38E251C40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8605E10-FB5E-48B2-8086-4E264FC6E7DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="3030" windowWidth="28800" windowHeight="11385" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5595" yWindow="3375" windowWidth="28800" windowHeight="11385" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overlap calculator" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -190,9 +190,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -210,6 +207,9 @@
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,7 +596,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,348 +607,348 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
+        <v>20</v>
+      </c>
+      <c r="B2" s="5">
+        <f>2*A2*TAN($J$2/2)</f>
+        <v>23.094010767585029</v>
+      </c>
+      <c r="C2" s="5">
+        <f>B2/4*3</f>
+        <v>17.320508075688771</v>
+      </c>
+      <c r="D2" s="6">
+        <f>(B2-$I$7)/B2</f>
+        <v>0.13397459621556129</v>
+      </c>
+      <c r="E2" s="6">
+        <f>(C2-I$5*I$6)/C2</f>
+        <v>0.53811978464829935</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="5">
+        <v>60</v>
+      </c>
+      <c r="J2" s="5">
+        <f>I2/180*PI()</f>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>35</v>
       </c>
-      <c r="B2" s="6">
-        <f>2*A2*TAN($J$2/2)</f>
-        <v>50.857976960375261</v>
-      </c>
-      <c r="C2" s="6">
-        <f>B2/4*3</f>
-        <v>38.143482720281447</v>
-      </c>
-      <c r="D2" s="7">
-        <f>(B2-$I$7)/B2</f>
-        <v>0.44944723181153057</v>
-      </c>
-      <c r="E2" s="7">
-        <f>(C2-I$5*I$6)/C2</f>
-        <v>0.7902656121186783</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="6">
-        <v>72</v>
-      </c>
-      <c r="J2" s="6">
-        <f>I2/180*PI()</f>
-        <v>1.2566370614359172</v>
-      </c>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="B3" s="5">
+        <f>2*A3*TAN($J$2/2)</f>
+        <v>40.414518843273804</v>
+      </c>
+      <c r="C3" s="5">
+        <f>B3/4*3</f>
+        <v>30.310889132455351</v>
+      </c>
+      <c r="D3" s="6">
+        <f>(B3-$I$7)/B3</f>
+        <v>0.50512834069460644</v>
+      </c>
+      <c r="E3" s="6">
+        <f>(C3-I$5*I$6)/C3</f>
+        <v>0.73606844837045682</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>40</v>
       </c>
-      <c r="B3" s="6">
-        <f>2*A3*TAN($J$2/2)</f>
-        <v>58.123402240428874</v>
-      </c>
-      <c r="C3" s="6">
-        <f>B3/4*3</f>
-        <v>43.592551680321655</v>
-      </c>
-      <c r="D3" s="7">
-        <f>(B3-$I$7)/B3</f>
-        <v>0.5182663278350893</v>
-      </c>
-      <c r="E3" s="7">
-        <f>(C3-I$5*I$6)/C3</f>
-        <v>0.81648241060384352</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="B4" s="5">
+        <f>2*A4*TAN($J$2/2)</f>
+        <v>46.188021535170058</v>
+      </c>
+      <c r="C4" s="5">
+        <f>B4/4*3</f>
+        <v>34.641016151377542</v>
+      </c>
+      <c r="D4" s="6">
+        <f>(B4-$I$7)/B4</f>
+        <v>0.5669872981077807</v>
+      </c>
+      <c r="E4" s="6">
+        <f>(C4-I$5*I$6)/C4</f>
+        <v>0.76905989232414962</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>50</v>
       </c>
-      <c r="B4" s="6">
-        <f>2*A4*TAN($J$2/2)</f>
-        <v>72.654252800536085</v>
-      </c>
-      <c r="C4" s="6">
-        <f>B4/4*3</f>
-        <v>54.490689600402064</v>
-      </c>
-      <c r="D4" s="7">
-        <f>(B4-$I$7)/B4</f>
-        <v>0.61461306226807144</v>
-      </c>
-      <c r="E4" s="7">
-        <f>(C4-I$5*I$6)/C4</f>
-        <v>0.85318592848307484</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>60</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <f>2*A5*TAN($J$2/2)</f>
-        <v>87.185103360643311</v>
-      </c>
-      <c r="C5" s="6">
+        <v>57.735026918962575</v>
+      </c>
+      <c r="C5" s="5">
         <f>B5/4*3</f>
-        <v>65.388827520482479</v>
-      </c>
-      <c r="D5" s="7">
+        <v>43.301270189221931</v>
+      </c>
+      <c r="D5" s="6">
         <f>(B5-$I$7)/B5</f>
-        <v>0.67884421855672616</v>
-      </c>
-      <c r="E5" s="7">
+        <v>0.65358983848622454</v>
+      </c>
+      <c r="E5" s="6">
         <f>(C5-I$5*I$6)/C5</f>
-        <v>0.87765494040256231</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4" t="s">
+        <v>0.81524791385931972</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>4</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>70</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <f>2*A6*TAN($J$2/2)</f>
-        <v>101.71595392075052</v>
-      </c>
-      <c r="C6" s="6">
+        <v>80.829037686547608</v>
+      </c>
+      <c r="C6" s="5">
         <f>B6/4*3</f>
-        <v>76.286965440562895</v>
-      </c>
-      <c r="D6" s="7">
+        <v>60.621778264910702</v>
+      </c>
+      <c r="D6" s="6">
         <f>(B6-$I$7)/B6</f>
-        <v>0.72472361590576528</v>
-      </c>
-      <c r="E6" s="7">
+        <v>0.75256417034730327</v>
+      </c>
+      <c r="E6" s="6">
         <f>(C6-I$5*I$6)/C6</f>
-        <v>0.8951328060593392</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4" t="s">
+        <v>0.86803422418522835</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>2</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="4"/>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="6">
-        <v>28</v>
-      </c>
-      <c r="J7" s="4" t="s">
+      <c r="I7" s="5">
+        <v>20</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="4"/>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>15</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="4"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>500</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>500</v>
       </c>
-      <c r="K10" s="4"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="5">
         <v>2700</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="4"/>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" ht="39" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <v>0.75</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="5">
         <f>H16*I5*I8*60/I7</f>
-        <v>96.428571428571431</v>
-      </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+        <v>135</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>